<commit_message>
raíz cuadrada, muestra resultado en pantalla
</commit_message>
<xml_diff>
--- a/bit-map.xlsx
+++ b/bit-map.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Esteban\Downloads\-CODE-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A1225E-E8B4-44F6-9875-E5DBEB6DF195}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2035B17A-BA47-4A11-93F6-791E5E9081F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{7D12F5E3-974F-4BA7-9E4E-83979BA242C7}"/>
   </bookViews>
@@ -53,7 +53,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="0_ ;\-0\ "/>
+    <numFmt numFmtId="164" formatCode="0_ ;\-0\ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -232,35 +232,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -599,13 +599,13 @@
   <dimension ref="A1:Z17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AA3" sqref="AA3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="3.5703125" defaultRowHeight="19.5" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="18" width="3.5703125" style="1"/>
-    <col min="21" max="21" width="21.42578125" style="11" customWidth="1"/>
+    <col min="21" max="21" width="38.5703125" style="2" customWidth="1"/>
     <col min="22" max="22" width="3.5703125" style="1"/>
     <col min="23" max="24" width="10.7109375" style="1" customWidth="1"/>
     <col min="27" max="16384" width="3.5703125" style="1"/>
@@ -660,7 +660,7 @@
       <c r="Q1" s="1">
         <v>16</v>
       </c>
-      <c r="U1" s="11" t="s">
+      <c r="U1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="W1" s="1" t="s">
@@ -674,28 +674,60 @@
       <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4"/>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
-      <c r="M2" s="4"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="4"/>
-      <c r="P2" s="4"/>
-      <c r="Q2" s="5"/>
-      <c r="U2" s="11">
-        <f>B2*1 + C2*10^1 + D2*10^2 + E2*10^3 + F2*10^4 + G2*10^5 +H2*10^6+I2*10^7+J2*10^8+K2*10^9+L2*10^10+M2*10^11+N2*10^12+O2*10^13+P2*10^14</f>
-        <v>0</v>
+      <c r="B2" s="3">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4">
+        <v>0</v>
+      </c>
+      <c r="D2" s="4">
+        <v>0</v>
+      </c>
+      <c r="E2" s="4">
+        <v>0</v>
+      </c>
+      <c r="F2" s="4">
+        <v>0</v>
+      </c>
+      <c r="G2" s="4">
+        <v>0</v>
+      </c>
+      <c r="H2" s="4">
+        <v>0</v>
+      </c>
+      <c r="I2" s="4">
+        <v>0</v>
+      </c>
+      <c r="J2" s="4">
+        <v>0</v>
+      </c>
+      <c r="K2" s="4">
+        <v>0</v>
+      </c>
+      <c r="L2" s="4">
+        <v>0</v>
+      </c>
+      <c r="M2" s="4">
+        <v>0</v>
+      </c>
+      <c r="N2" s="4">
+        <v>0</v>
+      </c>
+      <c r="O2" s="4">
+        <v>0</v>
+      </c>
+      <c r="P2" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>0</v>
+      </c>
+      <c r="U2" s="2" t="str">
+        <f>_xlfn.CONCAT(B2,C2,D2,E2,F2,G2,H2,I2,J2,K2,L2,M2,N2,O2,P2,Q2)</f>
+        <v>0000000000000000</v>
       </c>
       <c r="W2" s="1">
-        <f>B2*1 + C2*2^1 + D2*2^2 + E2*2^3 + F2*2^4 + G2*2^5 +H2*2^6+I2*2^7+J2*2^8+K2*2^9+L2*2^10+M2*2^11+N2*2^12+O2*2^13+P2*2^14</f>
+        <f t="shared" ref="W2:W17" si="0">B2*1 + C2*2^1 + D2*2^2 + E2*2^3 + F2*2^4 + G2*2^5 +H2*2^6+I2*2^7+J2*2^8+K2*2^9+L2*2^10+M2*2^11+N2*2^12+O2*2^13+P2*2^14</f>
         <v>0</v>
       </c>
       <c r="X2" s="1">
@@ -706,40 +738,60 @@
       <c r="A3" s="1">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2">
-        <v>1</v>
-      </c>
-      <c r="H3" s="2">
-        <v>1</v>
-      </c>
-      <c r="I3" s="2">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2">
-        <v>1</v>
-      </c>
-      <c r="K3" s="2">
-        <v>1</v>
-      </c>
-      <c r="L3" s="2">
-        <v>1</v>
-      </c>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="7"/>
-      <c r="U3" s="11">
-        <f>B3*1 + C3*10^1 + D3*10^2 + E3*10^3 + F3*10^4 + G3*10^5 +H3*10^6+I3*10^7+J3*10^8+K3*10^9+L3*10^10+M3*10^11+N3*10^12+O3*10^13+P3*10^14</f>
-        <v>11111100000</v>
+      <c r="B3" s="6">
+        <v>0</v>
+      </c>
+      <c r="C3" s="7">
+        <v>0</v>
+      </c>
+      <c r="D3" s="7">
+        <v>0</v>
+      </c>
+      <c r="E3" s="7">
+        <v>0</v>
+      </c>
+      <c r="F3" s="7">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>1</v>
+      </c>
+      <c r="H3" s="7">
+        <v>1</v>
+      </c>
+      <c r="I3" s="7">
+        <v>1</v>
+      </c>
+      <c r="J3" s="7">
+        <v>1</v>
+      </c>
+      <c r="K3" s="7">
+        <v>1</v>
+      </c>
+      <c r="L3" s="7">
+        <v>1</v>
+      </c>
+      <c r="M3" s="7">
+        <v>0</v>
+      </c>
+      <c r="N3" s="7">
+        <v>0</v>
+      </c>
+      <c r="O3" s="7">
+        <v>0</v>
+      </c>
+      <c r="P3" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>0</v>
+      </c>
+      <c r="U3" s="2" t="str">
+        <f t="shared" ref="U3:U17" si="1">_xlfn.CONCAT(B3,C3,D3,E3,F3,G3,H3,I3,J3,K3,L3,M3,N3,O3,P3,Q3)</f>
+        <v>0000011111100000</v>
       </c>
       <c r="W3" s="1">
-        <f>B3*1 + C3*2^1 + D3*2^2 + E3*2^3 + F3*2^4 + G3*2^5 +H3*2^6+I3*2^7+J3*2^8+K3*2^9+L3*2^10+M3*2^11+N3*2^12+O3*2^13+P3*2^14</f>
+        <f t="shared" si="0"/>
         <v>2016</v>
       </c>
       <c r="X3" s="1">
@@ -751,40 +803,64 @@
       <c r="A4" s="1">
         <v>3</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="2">
-        <v>1</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2">
-        <v>1</v>
-      </c>
-      <c r="M4" s="2">
-        <v>1</v>
-      </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="7"/>
-      <c r="U4" s="11">
-        <f>B4*1 + C4*10^1 + D4*10^2 + E4*10^3 + F4*10^4 + G4*10^5 +H4*10^6+I4*10^7+J4*10^8+K4*10^9+L4*10^10+M4*10^11+N4*10^12+O4*10^13+P4*10^14</f>
-        <v>110000110000</v>
+      <c r="B4" s="6">
+        <v>0</v>
+      </c>
+      <c r="C4" s="7">
+        <v>0</v>
+      </c>
+      <c r="D4" s="7">
+        <v>0</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0</v>
+      </c>
+      <c r="F4" s="7">
+        <v>1</v>
+      </c>
+      <c r="G4" s="7">
+        <v>1</v>
+      </c>
+      <c r="H4" s="7">
+        <v>0</v>
+      </c>
+      <c r="I4" s="7">
+        <v>0</v>
+      </c>
+      <c r="J4" s="7">
+        <v>0</v>
+      </c>
+      <c r="K4" s="7">
+        <v>0</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1</v>
+      </c>
+      <c r="N4" s="7">
+        <v>0</v>
+      </c>
+      <c r="O4" s="7">
+        <v>0</v>
+      </c>
+      <c r="P4" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>0</v>
+      </c>
+      <c r="U4" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0000110000110000</v>
       </c>
       <c r="W4" s="1">
-        <f>B4*1 + C4*2^1 + D4*2^2 + E4*2^3 + F4*2^4 + G4*2^5 +H4*2^6+I4*2^7+J4*2^8+K4*2^9+L4*2^10+M4*2^11+N4*2^12+O4*2^13+P4*2^14</f>
+        <f t="shared" si="0"/>
         <v>3120</v>
       </c>
       <c r="X4" s="1">
-        <f t="shared" ref="X4:X17" si="0">X3+32</f>
+        <f t="shared" ref="X4:X17" si="2">X3+32</f>
         <v>16448</v>
       </c>
     </row>
@@ -792,36 +868,64 @@
       <c r="A5" s="1">
         <v>4</v>
       </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2">
-        <v>1</v>
-      </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="7"/>
-      <c r="U5" s="11">
-        <f>B5*1 + C5*10^1 + D5*10^2 + E5*10^3 + F5*10^4 + G5*10^5 +H5*10^6+I5*10^7+J5*10^8+K5*10^9+L5*10^10+M5*10^11+N5*10^12+O5*10^13+P5*10^14</f>
-        <v>100000010000</v>
+      <c r="B5" s="6">
+        <v>0</v>
+      </c>
+      <c r="C5" s="7">
+        <v>0</v>
+      </c>
+      <c r="D5" s="7">
+        <v>0</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="7">
+        <v>1</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="7">
+        <v>0</v>
+      </c>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
+      <c r="M5" s="7">
+        <v>1</v>
+      </c>
+      <c r="N5" s="7">
+        <v>0</v>
+      </c>
+      <c r="O5" s="7">
+        <v>0</v>
+      </c>
+      <c r="P5" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>0</v>
+      </c>
+      <c r="U5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0000100000010000</v>
       </c>
       <c r="W5" s="1">
-        <f>B5*1 + C5*2^1 + D5*2^2 + E5*2^3 + F5*2^4 + G5*2^5 +H5*2^6+I5*2^7+J5*2^8+K5*2^9+L5*2^10+M5*2^11+N5*2^12+O5*2^13+P5*2^14</f>
+        <f t="shared" si="0"/>
         <v>2064</v>
       </c>
       <c r="X5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16480</v>
       </c>
     </row>
@@ -829,44 +933,64 @@
       <c r="A6" s="1">
         <v>5</v>
       </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="2">
-        <v>1</v>
-      </c>
-      <c r="G6" s="2">
-        <v>1</v>
-      </c>
-      <c r="H6" s="2">
-        <v>1</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2">
-        <v>1</v>
-      </c>
-      <c r="N6" s="2">
-        <v>1</v>
-      </c>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="7"/>
-      <c r="U6" s="11">
-        <f>B6*1 + C6*10^1 + D6*10^2 + E6*10^3 + F6*10^4 + G6*10^5 +H6*10^6+I6*10^7+J6*10^8+K6*10^9+L6*10^10+M6*10^11+N6*10^12+O6*10^13+P6*10^14</f>
-        <v>1100001111000</v>
+      <c r="B6" s="6">
+        <v>0</v>
+      </c>
+      <c r="C6" s="7">
+        <v>0</v>
+      </c>
+      <c r="D6" s="7">
+        <v>0</v>
+      </c>
+      <c r="E6" s="7">
+        <v>1</v>
+      </c>
+      <c r="F6" s="7">
+        <v>1</v>
+      </c>
+      <c r="G6" s="7">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7">
+        <v>1</v>
+      </c>
+      <c r="I6" s="7">
+        <v>0</v>
+      </c>
+      <c r="J6" s="7">
+        <v>0</v>
+      </c>
+      <c r="K6" s="7">
+        <v>0</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0</v>
+      </c>
+      <c r="M6" s="7">
+        <v>1</v>
+      </c>
+      <c r="N6" s="7">
+        <v>1</v>
+      </c>
+      <c r="O6" s="7">
+        <v>0</v>
+      </c>
+      <c r="P6" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>0</v>
+      </c>
+      <c r="U6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0001111000011000</v>
       </c>
       <c r="W6" s="1">
-        <f>B6*1 + C6*2^1 + D6*2^2 + E6*2^3 + F6*2^4 + G6*2^5 +H6*2^6+I6*2^7+J6*2^8+K6*2^9+L6*2^10+M6*2^11+N6*2^12+O6*2^13+P6*2^14</f>
+        <f t="shared" si="0"/>
         <v>6264</v>
       </c>
       <c r="X6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16512</v>
       </c>
     </row>
@@ -874,40 +998,64 @@
       <c r="A7" s="1">
         <v>6</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2">
-        <v>1</v>
-      </c>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2">
-        <v>1</v>
-      </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2">
-        <v>1</v>
-      </c>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="7"/>
-      <c r="U7" s="11">
-        <f>B7*1 + C7*10^1 + D7*10^2 + E7*10^3 + F7*10^4 + G7*10^5 +H7*10^6+I7*10^7+J7*10^8+K7*10^9+L7*10^10+M7*10^11+N7*10^12+O7*10^13+P7*10^14</f>
-        <v>10100010000100</v>
+      <c r="B7" s="6">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="7">
+        <v>0</v>
+      </c>
+      <c r="F7" s="7">
+        <v>0</v>
+      </c>
+      <c r="G7" s="7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="7">
+        <v>1</v>
+      </c>
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
+      <c r="M7" s="7">
+        <v>1</v>
+      </c>
+      <c r="N7" s="7">
+        <v>0</v>
+      </c>
+      <c r="O7" s="7">
+        <v>1</v>
+      </c>
+      <c r="P7" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>0</v>
+      </c>
+      <c r="U7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0010000100010100</v>
       </c>
       <c r="W7" s="1">
-        <f>B7*1 + C7*2^1 + D7*2^2 + E7*2^3 + F7*2^4 + G7*2^5 +H7*2^6+I7*2^7+J7*2^8+K7*2^9+L7*2^10+M7*2^11+N7*2^12+O7*2^13+P7*2^14</f>
+        <f t="shared" si="0"/>
         <v>10372</v>
       </c>
       <c r="X7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16544</v>
       </c>
     </row>
@@ -915,40 +1063,64 @@
       <c r="A8" s="1">
         <v>7</v>
       </c>
-      <c r="B8" s="6"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2">
-        <v>1</v>
-      </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2">
-        <v>1</v>
-      </c>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2">
-        <v>1</v>
-      </c>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2">
-        <v>1</v>
-      </c>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="7"/>
-      <c r="U8" s="11">
-        <f>B8*1 + C8*10^1 + D8*10^2 + E8*10^3 + F8*10^4 + G8*10^5 +H8*10^6+I8*10^7+J8*10^8+K8*10^9+L8*10^10+M8*10^11+N8*10^12+O8*10^13+P8*10^14</f>
-        <v>10100010000100</v>
+      <c r="B8" s="6">
+        <v>0</v>
+      </c>
+      <c r="C8" s="7">
+        <v>0</v>
+      </c>
+      <c r="D8" s="7">
+        <v>1</v>
+      </c>
+      <c r="E8" s="7">
+        <v>0</v>
+      </c>
+      <c r="F8" s="7">
+        <v>0</v>
+      </c>
+      <c r="G8" s="7">
+        <v>0</v>
+      </c>
+      <c r="H8" s="7">
+        <v>0</v>
+      </c>
+      <c r="I8" s="7">
+        <v>1</v>
+      </c>
+      <c r="J8" s="7">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <v>0</v>
+      </c>
+      <c r="L8" s="7">
+        <v>0</v>
+      </c>
+      <c r="M8" s="7">
+        <v>1</v>
+      </c>
+      <c r="N8" s="7">
+        <v>0</v>
+      </c>
+      <c r="O8" s="7">
+        <v>1</v>
+      </c>
+      <c r="P8" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>0</v>
+      </c>
+      <c r="U8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0010000100010100</v>
       </c>
       <c r="W8" s="1">
-        <f>B8*1 + C8*2^1 + D8*2^2 + E8*2^3 + F8*2^4 + G8*2^5 +H8*2^6+I8*2^7+J8*2^8+K8*2^9+L8*2^10+M8*2^11+N8*2^12+O8*2^13+P8*2^14</f>
+        <f t="shared" si="0"/>
         <v>10372</v>
       </c>
       <c r="X8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16576</v>
       </c>
     </row>
@@ -956,44 +1128,64 @@
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="6"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2">
-        <v>1</v>
-      </c>
-      <c r="F9" s="2">
-        <v>1</v>
-      </c>
-      <c r="G9" s="2">
-        <v>1</v>
-      </c>
-      <c r="H9" s="2">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2">
-        <v>1</v>
-      </c>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2">
-        <v>1</v>
-      </c>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="7"/>
-      <c r="U9" s="11">
-        <f>B9*1 + C9*10^1 + D9*10^2 + E9*10^3 + F9*10^4 + G9*10^5 +H9*10^6+I9*10^7+J9*10^8+K9*10^9+L9*10^10+M9*10^11+N9*10^12+O9*10^13+P9*10^14</f>
-        <v>10100001111000</v>
+      <c r="B9" s="6">
+        <v>0</v>
+      </c>
+      <c r="C9" s="7">
+        <v>0</v>
+      </c>
+      <c r="D9" s="7">
+        <v>0</v>
+      </c>
+      <c r="E9" s="7">
+        <v>1</v>
+      </c>
+      <c r="F9" s="7">
+        <v>1</v>
+      </c>
+      <c r="G9" s="7">
+        <v>1</v>
+      </c>
+      <c r="H9" s="7">
+        <v>1</v>
+      </c>
+      <c r="I9" s="7">
+        <v>0</v>
+      </c>
+      <c r="J9" s="7">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7">
+        <v>0</v>
+      </c>
+      <c r="L9" s="7">
+        <v>0</v>
+      </c>
+      <c r="M9" s="7">
+        <v>1</v>
+      </c>
+      <c r="N9" s="7">
+        <v>0</v>
+      </c>
+      <c r="O9" s="7">
+        <v>1</v>
+      </c>
+      <c r="P9" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="8">
+        <v>0</v>
+      </c>
+      <c r="U9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0001111000010100</v>
       </c>
       <c r="W9" s="1">
-        <f>B9*1 + C9*2^1 + D9*2^2 + E9*2^3 + F9*2^4 + G9*2^5 +H9*2^6+I9*2^7+J9*2^8+K9*2^9+L9*2^10+M9*2^11+N9*2^12+O9*2^13+P9*2^14</f>
+        <f t="shared" si="0"/>
         <v>10360</v>
       </c>
       <c r="X9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16608</v>
       </c>
     </row>
@@ -1001,38 +1193,64 @@
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="6"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2">
-        <v>1</v>
-      </c>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2">
-        <v>1</v>
-      </c>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2">
-        <v>1</v>
-      </c>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="7"/>
-      <c r="U10" s="11">
-        <f>B10*1 + C10*10^1 + D10*10^2 + E10*10^3 + F10*10^4 + G10*10^5 +H10*10^6+I10*10^7+J10*10^8+K10*10^9+L10*10^10+M10*10^11+N10*10^12+O10*10^13+P10*10^14</f>
-        <v>10100000010000</v>
+      <c r="B10" s="6">
+        <v>0</v>
+      </c>
+      <c r="C10" s="7">
+        <v>0</v>
+      </c>
+      <c r="D10" s="7">
+        <v>0</v>
+      </c>
+      <c r="E10" s="7">
+        <v>0</v>
+      </c>
+      <c r="F10" s="7">
+        <v>1</v>
+      </c>
+      <c r="G10" s="7">
+        <v>0</v>
+      </c>
+      <c r="H10" s="7">
+        <v>0</v>
+      </c>
+      <c r="I10" s="7">
+        <v>0</v>
+      </c>
+      <c r="J10" s="7">
+        <v>0</v>
+      </c>
+      <c r="K10" s="7">
+        <v>0</v>
+      </c>
+      <c r="L10" s="7">
+        <v>0</v>
+      </c>
+      <c r="M10" s="7">
+        <v>1</v>
+      </c>
+      <c r="N10" s="7">
+        <v>0</v>
+      </c>
+      <c r="O10" s="7">
+        <v>1</v>
+      </c>
+      <c r="P10" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q10" s="8">
+        <v>0</v>
+      </c>
+      <c r="U10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0000100000010100</v>
       </c>
       <c r="W10" s="1">
-        <f>B10*1 + C10*2^1 + D10*2^2 + E10*2^3 + F10*2^4 + G10*2^5 +H10*2^6+I10*2^7+J10*2^8+K10*2^9+L10*2^10+M10*2^11+N10*2^12+O10*2^13+P10*2^14</f>
+        <f t="shared" si="0"/>
         <v>10256</v>
       </c>
       <c r="X10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16640</v>
       </c>
     </row>
@@ -1040,38 +1258,64 @@
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2">
-        <v>1</v>
-      </c>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2">
-        <v>1</v>
-      </c>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2">
-        <v>1</v>
-      </c>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="7"/>
-      <c r="U11" s="11">
-        <f>B11*1 + C11*10^1 + D11*10^2 + E11*10^3 + F11*10^4 + G11*10^5 +H11*10^6+I11*10^7+J11*10^8+K11*10^9+L11*10^10+M11*10^11+N11*10^12+O11*10^13+P11*10^14</f>
-        <v>10100000010000</v>
+      <c r="B11" s="6">
+        <v>0</v>
+      </c>
+      <c r="C11" s="7">
+        <v>0</v>
+      </c>
+      <c r="D11" s="7">
+        <v>0</v>
+      </c>
+      <c r="E11" s="7">
+        <v>0</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="7">
+        <v>0</v>
+      </c>
+      <c r="H11" s="7">
+        <v>0</v>
+      </c>
+      <c r="I11" s="7">
+        <v>0</v>
+      </c>
+      <c r="J11" s="7">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <v>0</v>
+      </c>
+      <c r="L11" s="7">
+        <v>0</v>
+      </c>
+      <c r="M11" s="7">
+        <v>1</v>
+      </c>
+      <c r="N11" s="7">
+        <v>0</v>
+      </c>
+      <c r="O11" s="7">
+        <v>1</v>
+      </c>
+      <c r="P11" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="8">
+        <v>0</v>
+      </c>
+      <c r="U11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0000100000010100</v>
       </c>
       <c r="W11" s="1">
-        <f>B11*1 + C11*2^1 + D11*2^2 + E11*2^3 + F11*2^4 + G11*2^5 +H11*2^6+I11*2^7+J11*2^8+K11*2^9+L11*2^10+M11*2^11+N11*2^12+O11*2^13+P11*2^14</f>
+        <f t="shared" si="0"/>
         <v>10256</v>
       </c>
       <c r="X11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16672</v>
       </c>
     </row>
@@ -1079,38 +1323,64 @@
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2">
-        <v>1</v>
-      </c>
-      <c r="N12" s="2">
-        <v>1</v>
-      </c>
-      <c r="O12" s="2"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="7"/>
-      <c r="U12" s="11">
-        <f>B12*1 + C12*10^1 + D12*10^2 + E12*10^3 + F12*10^4 + G12*10^5 +H12*10^6+I12*10^7+J12*10^8+K12*10^9+L12*10^10+M12*10^11+N12*10^12+O12*10^13+P12*10^14</f>
-        <v>1100000010000</v>
+      <c r="B12" s="6">
+        <v>0</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0</v>
+      </c>
+      <c r="M12" s="7">
+        <v>1</v>
+      </c>
+      <c r="N12" s="7">
+        <v>1</v>
+      </c>
+      <c r="O12" s="7">
+        <v>0</v>
+      </c>
+      <c r="P12" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="8">
+        <v>0</v>
+      </c>
+      <c r="U12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0000100000011000</v>
       </c>
       <c r="W12" s="1">
-        <f>B12*1 + C12*2^1 + D12*2^2 + E12*2^3 + F12*2^4 + G12*2^5 +H12*2^6+I12*2^7+J12*2^8+K12*2^9+L12*2^10+M12*2^11+N12*2^12+O12*2^13+P12*2^14</f>
+        <f t="shared" si="0"/>
         <v>6160</v>
       </c>
       <c r="X12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16704</v>
       </c>
     </row>
@@ -1118,40 +1388,64 @@
       <c r="A13" s="1">
         <v>12</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2">
-        <v>1</v>
-      </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2">
-        <v>1</v>
-      </c>
-      <c r="J13" s="2">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2">
-        <v>1</v>
-      </c>
-      <c r="N13" s="2"/>
-      <c r="O13" s="2"/>
-      <c r="P13" s="2"/>
-      <c r="Q13" s="7"/>
-      <c r="U13" s="11">
-        <f>B13*1 + C13*10^1 + D13*10^2 + E13*10^3 + F13*10^4 + G13*10^5 +H13*10^6+I13*10^7+J13*10^8+K13*10^9+L13*10^10+M13*10^11+N13*10^12+O13*10^13+P13*10^14</f>
-        <v>100110010000</v>
+      <c r="B13" s="6">
+        <v>0</v>
+      </c>
+      <c r="C13" s="7">
+        <v>0</v>
+      </c>
+      <c r="D13" s="7">
+        <v>0</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="7">
+        <v>1</v>
+      </c>
+      <c r="G13" s="7">
+        <v>0</v>
+      </c>
+      <c r="H13" s="7">
+        <v>0</v>
+      </c>
+      <c r="I13" s="7">
+        <v>1</v>
+      </c>
+      <c r="J13" s="7">
+        <v>1</v>
+      </c>
+      <c r="K13" s="7">
+        <v>0</v>
+      </c>
+      <c r="L13" s="7">
+        <v>0</v>
+      </c>
+      <c r="M13" s="7">
+        <v>1</v>
+      </c>
+      <c r="N13" s="7">
+        <v>0</v>
+      </c>
+      <c r="O13" s="7">
+        <v>0</v>
+      </c>
+      <c r="P13" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="8">
+        <v>0</v>
+      </c>
+      <c r="U13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0000100110010000</v>
       </c>
       <c r="W13" s="1">
-        <f>B13*1 + C13*2^1 + D13*2^2 + E13*2^3 + F13*2^4 + G13*2^5 +H13*2^6+I13*2^7+J13*2^8+K13*2^9+L13*2^10+M13*2^11+N13*2^12+O13*2^13+P13*2^14</f>
+        <f t="shared" si="0"/>
         <v>2448</v>
       </c>
       <c r="X13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16736</v>
       </c>
     </row>
@@ -1159,40 +1453,64 @@
       <c r="A14" s="1">
         <v>13</v>
       </c>
-      <c r="B14" s="6"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2">
-        <v>1</v>
-      </c>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2">
-        <v>1</v>
-      </c>
-      <c r="N14" s="2"/>
-      <c r="O14" s="2"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="7"/>
-      <c r="U14" s="11">
-        <f>B14*1 + C14*10^1 + D14*10^2 + E14*10^3 + F14*10^4 + G14*10^5 +H14*10^6+I14*10^7+J14*10^8+K14*10^9+L14*10^10+M14*10^11+N14*10^12+O14*10^13+P14*10^14</f>
-        <v>101001010000</v>
+      <c r="B14" s="6">
+        <v>0</v>
+      </c>
+      <c r="C14" s="7">
+        <v>0</v>
+      </c>
+      <c r="D14" s="7">
+        <v>0</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0</v>
+      </c>
+      <c r="F14" s="7">
+        <v>1</v>
+      </c>
+      <c r="G14" s="7">
+        <v>0</v>
+      </c>
+      <c r="H14" s="7">
+        <v>1</v>
+      </c>
+      <c r="I14" s="7">
+        <v>0</v>
+      </c>
+      <c r="J14" s="7">
+        <v>0</v>
+      </c>
+      <c r="K14" s="7">
+        <v>1</v>
+      </c>
+      <c r="L14" s="7">
+        <v>0</v>
+      </c>
+      <c r="M14" s="7">
+        <v>1</v>
+      </c>
+      <c r="N14" s="7">
+        <v>0</v>
+      </c>
+      <c r="O14" s="7">
+        <v>0</v>
+      </c>
+      <c r="P14" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="8">
+        <v>0</v>
+      </c>
+      <c r="U14" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0000101001010000</v>
       </c>
       <c r="W14" s="1">
-        <f>B14*1 + C14*2^1 + D14*2^2 + E14*2^3 + F14*2^4 + G14*2^5 +H14*2^6+I14*2^7+J14*2^8+K14*2^9+L14*2^10+M14*2^11+N14*2^12+O14*2^13+P14*2^14</f>
+        <f t="shared" si="0"/>
         <v>2640</v>
       </c>
       <c r="X14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16768</v>
       </c>
     </row>
@@ -1200,40 +1518,64 @@
       <c r="A15" s="1">
         <v>14</v>
       </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2">
-        <v>1</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2">
-        <v>1</v>
-      </c>
-      <c r="L15" s="2">
-        <v>1</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="2"/>
-      <c r="O15" s="2"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="7"/>
-      <c r="U15" s="11">
-        <f>B15*1 + C15*10^1 + D15*10^2 + E15*10^3 + F15*10^4 + G15*10^5 +H15*10^6+I15*10^7+J15*10^8+K15*10^9+L15*10^10+M15*10^11+N15*10^12+O15*10^13+P15*10^14</f>
-        <v>11001100000</v>
+      <c r="B15" s="6">
+        <v>0</v>
+      </c>
+      <c r="C15" s="7">
+        <v>0</v>
+      </c>
+      <c r="D15" s="7">
+        <v>0</v>
+      </c>
+      <c r="E15" s="7">
+        <v>0</v>
+      </c>
+      <c r="F15" s="7">
+        <v>0</v>
+      </c>
+      <c r="G15" s="7">
+        <v>1</v>
+      </c>
+      <c r="H15" s="7">
+        <v>1</v>
+      </c>
+      <c r="I15" s="7">
+        <v>0</v>
+      </c>
+      <c r="J15" s="7">
+        <v>0</v>
+      </c>
+      <c r="K15" s="7">
+        <v>1</v>
+      </c>
+      <c r="L15" s="7">
+        <v>1</v>
+      </c>
+      <c r="M15" s="7">
+        <v>0</v>
+      </c>
+      <c r="N15" s="7">
+        <v>0</v>
+      </c>
+      <c r="O15" s="7">
+        <v>0</v>
+      </c>
+      <c r="P15" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="8">
+        <v>0</v>
+      </c>
+      <c r="U15" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0000011001100000</v>
       </c>
       <c r="W15" s="1">
-        <f>B15*1 + C15*2^1 + D15*2^2 + E15*2^3 + F15*2^4 + G15*2^5 +H15*2^6+I15*2^7+J15*2^8+K15*2^9+L15*2^10+M15*2^11+N15*2^12+O15*2^13+P15*2^14</f>
+        <f t="shared" si="0"/>
         <v>1632</v>
       </c>
       <c r="X15" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16800</v>
       </c>
     </row>
@@ -1241,32 +1583,64 @@
       <c r="A16" s="1">
         <v>15</v>
       </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="2"/>
-      <c r="O16" s="2"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="7"/>
-      <c r="U16" s="11">
-        <f>B16*1 + C16*10^1 + D16*10^2 + E16*10^3 + F16*10^4 + G16*10^5 +H16*10^6+I16*10^7+J16*10^8+K16*10^9+L16*10^10+M16*10^11+N16*10^12+O16*10^13+P16*10^14</f>
-        <v>0</v>
+      <c r="B16" s="6">
+        <v>0</v>
+      </c>
+      <c r="C16" s="7">
+        <v>0</v>
+      </c>
+      <c r="D16" s="7">
+        <v>0</v>
+      </c>
+      <c r="E16" s="7">
+        <v>0</v>
+      </c>
+      <c r="F16" s="7">
+        <v>0</v>
+      </c>
+      <c r="G16" s="7">
+        <v>0</v>
+      </c>
+      <c r="H16" s="7">
+        <v>0</v>
+      </c>
+      <c r="I16" s="7">
+        <v>0</v>
+      </c>
+      <c r="J16" s="7">
+        <v>0</v>
+      </c>
+      <c r="K16" s="7">
+        <v>0</v>
+      </c>
+      <c r="L16" s="7">
+        <v>0</v>
+      </c>
+      <c r="M16" s="7">
+        <v>0</v>
+      </c>
+      <c r="N16" s="7">
+        <v>0</v>
+      </c>
+      <c r="O16" s="7">
+        <v>0</v>
+      </c>
+      <c r="P16" s="7">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>0</v>
+      </c>
+      <c r="U16" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0000000000000000</v>
       </c>
       <c r="W16" s="1">
-        <f>B16*1 + C16*2^1 + D16*2^2 + E16*2^3 + F16*2^4 + G16*2^5 +H16*2^6+I16*2^7+J16*2^8+K16*2^9+L16*2^10+M16*2^11+N16*2^12+O16*2^13+P16*2^14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X16" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16832</v>
       </c>
     </row>
@@ -1274,32 +1648,64 @@
       <c r="A17" s="1">
         <v>16</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="9"/>
-      <c r="M17" s="9"/>
-      <c r="N17" s="9"/>
-      <c r="O17" s="9"/>
-      <c r="P17" s="9"/>
-      <c r="Q17" s="10"/>
-      <c r="U17" s="11">
-        <f>B17*1 + C17*10^1 + D17*10^2 + E17*10^3 + F17*10^4 + G17*10^5 +H17*10^6+I17*10^7+J17*10^8+K17*10^9+L17*10^10+M17*10^11+N17*10^12+O17*10^13+P17*10^14</f>
-        <v>0</v>
+      <c r="B17" s="9">
+        <v>0</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0</v>
+      </c>
+      <c r="J17" s="10">
+        <v>0</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0</v>
+      </c>
+      <c r="L17" s="10">
+        <v>0</v>
+      </c>
+      <c r="M17" s="10">
+        <v>0</v>
+      </c>
+      <c r="N17" s="10">
+        <v>0</v>
+      </c>
+      <c r="O17" s="10">
+        <v>0</v>
+      </c>
+      <c r="P17" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="11">
+        <v>0</v>
+      </c>
+      <c r="U17" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>0000000000000000</v>
       </c>
       <c r="W17" s="1">
-        <f>B17*1 + C17*2^1 + D17*2^2 + E17*2^3 + F17*2^4 + G17*2^5 +H17*2^6+I17*2^7+J17*2^8+K17*2^9+L17*2^10+M17*2^11+N17*2^12+O17*2^13+P17*2^14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="X17" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>16864</v>
       </c>
     </row>

</xml_diff>